<commit_message>
update code, add check banner
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -626,10 +626,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
@@ -638,10 +638,10 @@
     <col width="35.85546875" customWidth="1" style="1" min="2" max="2"/>
     <col width="15.42578125" customWidth="1" style="1" min="3" max="3"/>
     <col width="34.42578125" customWidth="1" style="1" min="4" max="4"/>
-    <col hidden="1" width="14" customWidth="1" style="1" min="5" max="5"/>
-    <col hidden="1" width="23.7109375" customWidth="1" style="1" min="6" max="6"/>
-    <col hidden="1" width="8.85546875" customWidth="1" style="1" min="7" max="7"/>
-    <col hidden="1" width="56.28515625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="14" customWidth="1" style="1" min="5" max="5"/>
+    <col width="23.7109375" customWidth="1" style="1" min="6" max="6"/>
+    <col width="8.85546875" customWidth="1" style="1" min="7" max="7"/>
+    <col width="56.28515625" customWidth="1" style="1" min="8" max="8"/>
     <col width="44.28515625" customWidth="1" style="1" min="9" max="9"/>
     <col width="12" customWidth="1" style="1" min="10" max="10"/>
     <col width="59.7109375" customWidth="1" style="1" min="11" max="11"/>
@@ -1516,7 +1516,9 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="n"/>
+      <c r="A29" s="3" t="n">
+        <v>28</v>
+      </c>
       <c r="B29" s="20" t="n"/>
       <c r="C29" s="10" t="inlineStr">
         <is>
@@ -1544,8 +1546,569 @@
       </c>
     </row>
     <row r="30">
-      <c r="J30" t="inlineStr"/>
-      <c r="K30">
+      <c r="A30" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>画面の起動</t>
+        </is>
+      </c>
+      <c r="C30" s="10" t="inlineStr">
+        <is>
+          <t>画面起動</t>
+        </is>
+      </c>
+      <c r="D30" s="8" t="inlineStr">
+        <is>
+          <t>https://kakaku.com/</t>
+        </is>
+      </c>
+      <c r="E30" s="8" t="n"/>
+      <c r="F30" s="8" t="n"/>
+      <c r="G30" s="8" t="n"/>
+      <c r="H30" s="15" t="n"/>
+      <c r="I30" s="8" t="n"/>
+      <c r="J30" s="8" t="inlineStr"/>
+      <c r="K30" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1" s="21">
+      <c r="A31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 1</t>
+        </is>
+      </c>
+      <c r="C31" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D31" s="8" t="n"/>
+      <c r="E31" s="8" t="n"/>
+      <c r="F31" s="8" t="n"/>
+      <c r="G31" s="8" t="n"/>
+      <c r="H31" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[2]/div/a/span/div/img</t>
+        </is>
+      </c>
+      <c r="I31" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_admin.jpg", "banner_admin.jpg")</f>
+        <v/>
+      </c>
+      <c r="J31" s="8" t="inlineStr"/>
+      <c r="K31" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="20" t="n"/>
+      <c r="C32" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D32" s="8" t="n"/>
+      <c r="E32" s="8" t="n"/>
+      <c r="F32" s="8" t="n"/>
+      <c r="G32" s="8" t="n"/>
+      <c r="H32" s="15" t="n"/>
+      <c r="I32" s="8" t="n"/>
+      <c r="J32" s="8" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K32" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\14-Check Banner 1-False.png", "14-Check Banner 1-False.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" ht="15" customHeight="1" s="21">
+      <c r="A33" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 2</t>
+        </is>
+      </c>
+      <c r="C33" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D33" s="8" t="n"/>
+      <c r="E33" s="8" t="n"/>
+      <c r="F33" s="8" t="n"/>
+      <c r="G33" s="8" t="n"/>
+      <c r="H33" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[1]/div[1]/div[2]/div[2]/div[4]/div[2]/div/p/img</t>
+        </is>
+      </c>
+      <c r="I33" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_GTune_P5.jpg", "banner_GTune_P5.jpg")</f>
+        <v/>
+      </c>
+      <c r="J33" s="8" t="inlineStr"/>
+      <c r="K33" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="20" t="n"/>
+      <c r="C34" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D34" s="8" t="n"/>
+      <c r="E34" s="8" t="n"/>
+      <c r="F34" s="8" t="n"/>
+      <c r="G34" s="8" t="n"/>
+      <c r="H34" s="15" t="n"/>
+      <c r="I34" s="8" t="n"/>
+      <c r="J34" s="8" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K34" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\15-Check Banner 2-False.png", "15-Check Banner 2-False.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" ht="15" customHeight="1" s="21">
+      <c r="A35" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 3</t>
+        </is>
+      </c>
+      <c r="C35" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D35" s="8" t="n"/>
+      <c r="E35" s="8" t="n"/>
+      <c r="F35" s="8" t="n"/>
+      <c r="G35" s="8" t="n"/>
+      <c r="H35" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[1]/div[1]/div[2]/div[2]/div[4]/ul/li[1]/div/div/p/img</t>
+        </is>
+      </c>
+      <c r="I35" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_marumie.jpg", "banner_marumie.jpg")</f>
+        <v/>
+      </c>
+      <c r="J35" s="8" t="inlineStr"/>
+      <c r="K35" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="20" t="n"/>
+      <c r="C36" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D36" s="8" t="n"/>
+      <c r="E36" s="8" t="n"/>
+      <c r="F36" s="8" t="n"/>
+      <c r="G36" s="8" t="n"/>
+      <c r="H36" s="15" t="n"/>
+      <c r="I36" s="8" t="n"/>
+      <c r="J36" s="8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K36" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\16-Check Banner 3-True.png", "16-Check Banner 3-True.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" ht="15" customHeight="1" s="21">
+      <c r="A37" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 4</t>
+        </is>
+      </c>
+      <c r="C37" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D37" s="8" t="n"/>
+      <c r="E37" s="8" t="n"/>
+      <c r="F37" s="8" t="n"/>
+      <c r="G37" s="8" t="n"/>
+      <c r="H37" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[1]/div[1]/div[2]/div[2]/div[4]/ul/li[2]/div/div/p/img</t>
+        </is>
+      </c>
+      <c r="I37" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_feature.jpg", "banner_feature.jpg")</f>
+        <v/>
+      </c>
+      <c r="J37" s="8" t="inlineStr"/>
+      <c r="K37" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="20" t="n"/>
+      <c r="C38" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D38" s="8" t="n"/>
+      <c r="E38" s="8" t="n"/>
+      <c r="F38" s="8" t="n"/>
+      <c r="G38" s="8" t="n"/>
+      <c r="H38" s="15" t="n"/>
+      <c r="I38" s="8" t="n"/>
+      <c r="J38" s="8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K38" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\17-Check Banner 4-True.png", "17-Check Banner 4-True.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" ht="15" customHeight="1" s="21">
+      <c r="A39" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 5</t>
+        </is>
+      </c>
+      <c r="C39" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D39" s="8" t="n"/>
+      <c r="E39" s="8" t="n"/>
+      <c r="F39" s="8" t="n"/>
+      <c r="G39" s="8" t="n"/>
+      <c r="H39" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[1]/div[1]/div[2]/div[2]/div[4]/ul/li[3]/div/div/p/img</t>
+        </is>
+      </c>
+      <c r="I39" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_camera.jpg", "banner_camera.jpg")</f>
+        <v/>
+      </c>
+      <c r="J39" s="8" t="inlineStr"/>
+      <c r="K39" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="20" t="n"/>
+      <c r="C40" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D40" s="8" t="n"/>
+      <c r="E40" s="8" t="n"/>
+      <c r="F40" s="8" t="n"/>
+      <c r="G40" s="8" t="n"/>
+      <c r="H40" s="15" t="n"/>
+      <c r="I40" s="8" t="n"/>
+      <c r="J40" s="8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K40" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\18-Check Banner 5-True.png", "18-Check Banner 5-True.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" ht="15" customHeight="1" s="21">
+      <c r="A41" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 6</t>
+        </is>
+      </c>
+      <c r="C41" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D41" s="8" t="n"/>
+      <c r="E41" s="8" t="n"/>
+      <c r="F41" s="8" t="n"/>
+      <c r="G41" s="8" t="n"/>
+      <c r="H41" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[1]/div[1]/div[2]/div[2]/div[4]/ul/li[4]/div/div/p/img</t>
+        </is>
+      </c>
+      <c r="I41" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_houseware.png", "banner_houseware.png")</f>
+        <v/>
+      </c>
+      <c r="J41" s="8" t="inlineStr"/>
+      <c r="K41" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="20" t="n"/>
+      <c r="C42" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D42" s="8" t="n"/>
+      <c r="E42" s="8" t="n"/>
+      <c r="F42" s="8" t="n"/>
+      <c r="G42" s="8" t="n"/>
+      <c r="H42" s="15" t="n"/>
+      <c r="I42" s="8" t="n"/>
+      <c r="J42" s="8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K42" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\19-Check Banner 6-True.png", "19-Check Banner 6-True.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" ht="15" customHeight="1" s="21">
+      <c r="A43" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 7</t>
+        </is>
+      </c>
+      <c r="C43" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D43" s="8" t="n"/>
+      <c r="E43" s="8" t="n"/>
+      <c r="F43" s="8" t="n"/>
+      <c r="G43" s="8" t="n"/>
+      <c r="H43" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[1]/div[1]/div[2]/div[2]/div[4]/ul/li[5]/div/div/p/img</t>
+        </is>
+      </c>
+      <c r="I43" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_bag.png", "banner_bag.png")</f>
+        <v/>
+      </c>
+      <c r="J43" s="8" t="inlineStr"/>
+      <c r="K43" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="20" t="n"/>
+      <c r="C44" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D44" s="8" t="n"/>
+      <c r="E44" s="8" t="n"/>
+      <c r="F44" s="8" t="n"/>
+      <c r="G44" s="8" t="n"/>
+      <c r="H44" s="15" t="n"/>
+      <c r="I44" s="8" t="n"/>
+      <c r="J44" s="8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K44" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\20-Check Banner 7-True.png", "20-Check Banner 7-True.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" ht="15" customHeight="1" s="21">
+      <c r="A45" s="3" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 8</t>
+        </is>
+      </c>
+      <c r="C45" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D45" s="8" t="n"/>
+      <c r="E45" s="8" t="n"/>
+      <c r="F45" s="8" t="n"/>
+      <c r="G45" s="8" t="n"/>
+      <c r="H45" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[1]/div[1]/div[2]/div[2]/div[4]/ul/li[6]/div/div/p/img</t>
+        </is>
+      </c>
+      <c r="I45" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_newlife.png", "banner_newlife.png")</f>
+        <v/>
+      </c>
+      <c r="J45" s="8" t="inlineStr"/>
+      <c r="K45" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="20" t="n"/>
+      <c r="C46" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D46" s="8" t="n"/>
+      <c r="E46" s="8" t="n"/>
+      <c r="F46" s="8" t="n"/>
+      <c r="G46" s="8" t="n"/>
+      <c r="H46" s="15" t="n"/>
+      <c r="I46" s="8" t="n"/>
+      <c r="J46" s="8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K46" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\21-Check Banner 8-True.png", "21-Check Banner 8-True.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" ht="15" customHeight="1" s="21">
+      <c r="A47" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="20" t="inlineStr">
+        <is>
+          <t>Check Banner 9</t>
+        </is>
+      </c>
+      <c r="C47" s="10" t="inlineStr">
+        <is>
+          <t>Check banner</t>
+        </is>
+      </c>
+      <c r="D47" s="8" t="n"/>
+      <c r="E47" s="8" t="n"/>
+      <c r="F47" s="8" t="n"/>
+      <c r="G47" s="8" t="n"/>
+      <c r="H47" s="15" t="inlineStr">
+        <is>
+          <t>/html/body/div[1]/div[1]/div[2]/div[2]/div[4]/ul/li[7]/div/div/p/img</t>
+        </is>
+      </c>
+      <c r="I47" s="7">
+        <f>HYPERLINK("d:\TanLV\SS1\banner_image\banner_jalcard.jpg", "banner_jalcard.jpg")</f>
+        <v/>
+      </c>
+      <c r="J47" s="8" t="inlineStr"/>
+      <c r="K47" s="8">
+        <f>HYPERLINK("", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="20" t="n"/>
+      <c r="C48" s="10" t="inlineStr">
+        <is>
+          <t>Check the value</t>
+        </is>
+      </c>
+      <c r="D48" s="8" t="n"/>
+      <c r="E48" s="8" t="n"/>
+      <c r="F48" s="8" t="n"/>
+      <c r="G48" s="8" t="n"/>
+      <c r="H48" s="15" t="n"/>
+      <c r="I48" s="8" t="n"/>
+      <c r="J48" s="8" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K48" s="8">
+        <f>HYPERLINK("d:\TanLV\SS1\image\22-Check Banner 9-False.png", "22-Check Banner 9-False.png")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="J49" t="inlineStr"/>
+      <c r="K49">
         <f>HYPERLINK("", "")</f>
         <v/>
       </c>

</xml_diff>